<commit_message>
Explained the Amphenol DB25S064TLF
and added more sources and order numbers.
</commit_message>
<xml_diff>
--- a/Diag586220_Harness/C128_Keyboard_PCB/Rev. 1/Excel/C128_Diag_KeyB_BOM_v1_1.xlsx
+++ b/Diag586220_Harness/C128_Keyboard_PCB/Rev. 1/Excel/C128_Diag_KeyB_BOM_v1_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projekte\_Eigene\C64-Projects\Diag586220_Harness\C128_Keyboard_PCB\Rev. 1\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084C2F91-6D5D-4A06-B41B-A69B5ABD052C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4DA7AD-11A4-42E1-930E-6C992DE23730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2196" yWindow="756" windowWidth="25824" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4452" yWindow="1908" windowWidth="23040" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,15 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Stückliste!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -196,10 +205,6 @@
     <t>PCB Revision</t>
   </si>
   <si>
-    <t>DSub 25, female, solder cups, e.g. Reichelt.de: D-SUB BU 25. Recommended type: Amphenol DB25S064TLF (Digikey  
-609-1519-ND)</t>
-  </si>
-  <si>
     <t>Rev. 1.0 -&gt; 1.1</t>
   </si>
   <si>
@@ -207,19 +212,28 @@
   </si>
   <si>
     <t>Bill of Material Rev. 1.1</t>
+  </si>
+  <si>
+    <t>DSub 25, female, solder cups, strikly recommended type: Amphenol DB25S064TLF (Digikey 609-1519-ND, Farnell 2347730, Mouser 649-DB25S064TLF, Newark: 62K4006, Conrad.de: 1401537 - 62). Other might not connect the square pin header on the C128 mobo not well enough.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Futura Lt BT"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -706,49 +720,49 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -756,10 +770,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -771,34 +785,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1303,7 +1320,7 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,24 +1334,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="A2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1439,7 +1456,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="6" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1456,8 +1473,8 @@
       <c r="E8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>49</v>
+      <c r="F8" s="19" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -1632,21 +1649,21 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="3">
         <v>5</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>51</v>
+      <c r="C20" s="16" t="s">
+        <v>50</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="3"/>

</xml_diff>